<commit_message>
Major additions to & retooling of scoring
</commit_message>
<xml_diff>
--- a/testdata/NC20C_scores_SAMPLE.xlsx
+++ b/testdata/NC20C_scores_SAMPLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/rdaensemble/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3F4C2E-F9AC-1443-BB15-102F44068D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F582FAB-3637-D84C-8F1B-E219E919E7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="500" windowWidth="27080" windowHeight="16940" xr2:uid="{2772DF00-8910-C444-91D8-088A3495265C}"/>
   </bookViews>
@@ -994,10 +994,10 @@
   <dimension ref="A1:BF101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AR2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AW1" sqref="AW1:AW1048576"/>
+      <selection pane="bottomRight" activeCell="BA1" sqref="BA1:BA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1053,7 +1053,7 @@
     <col min="50" max="50" width="14.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="15" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="8" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="12.5" bestFit="1" customWidth="1"/>
@@ -1218,7 +1218,7 @@
       <c r="AZ1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="6" t="s">
+      <c r="BA1" s="5" t="s">
         <v>52</v>
       </c>
       <c r="BB1" s="6" t="s">
@@ -1394,7 +1394,7 @@
       <c r="AZ2">
         <v>64</v>
       </c>
-      <c r="BA2">
+      <c r="BA2" s="3">
         <v>53</v>
       </c>
       <c r="BB2">
@@ -1570,7 +1570,7 @@
       <c r="AZ3">
         <v>63</v>
       </c>
-      <c r="BA3">
+      <c r="BA3" s="3">
         <v>47</v>
       </c>
       <c r="BB3">
@@ -1746,7 +1746,7 @@
       <c r="AZ4">
         <v>58</v>
       </c>
-      <c r="BA4">
+      <c r="BA4" s="3">
         <v>52</v>
       </c>
       <c r="BB4">
@@ -1922,7 +1922,7 @@
       <c r="AZ5">
         <v>56</v>
       </c>
-      <c r="BA5">
+      <c r="BA5" s="3">
         <v>49</v>
       </c>
       <c r="BB5">
@@ -2098,7 +2098,7 @@
       <c r="AZ6">
         <v>56</v>
       </c>
-      <c r="BA6">
+      <c r="BA6" s="3">
         <v>45</v>
       </c>
       <c r="BB6">
@@ -2274,7 +2274,7 @@
       <c r="AZ7">
         <v>55</v>
       </c>
-      <c r="BA7">
+      <c r="BA7" s="3">
         <v>45</v>
       </c>
       <c r="BB7">
@@ -2450,7 +2450,7 @@
       <c r="AZ8">
         <v>53</v>
       </c>
-      <c r="BA8">
+      <c r="BA8" s="3">
         <v>48</v>
       </c>
       <c r="BB8">
@@ -2626,7 +2626,7 @@
       <c r="AZ9">
         <v>52</v>
       </c>
-      <c r="BA9">
+      <c r="BA9" s="3">
         <v>38</v>
       </c>
       <c r="BB9">
@@ -2802,7 +2802,7 @@
       <c r="AZ10">
         <v>49</v>
       </c>
-      <c r="BA10">
+      <c r="BA10" s="3">
         <v>38</v>
       </c>
       <c r="BB10">
@@ -2978,7 +2978,7 @@
       <c r="AZ11">
         <v>49</v>
       </c>
-      <c r="BA11">
+      <c r="BA11" s="3">
         <v>38</v>
       </c>
       <c r="BB11">
@@ -3154,7 +3154,7 @@
       <c r="AZ12">
         <v>47</v>
       </c>
-      <c r="BA12">
+      <c r="BA12" s="3">
         <v>37</v>
       </c>
       <c r="BB12">
@@ -3330,7 +3330,7 @@
       <c r="AZ13">
         <v>47</v>
       </c>
-      <c r="BA13">
+      <c r="BA13" s="3">
         <v>40</v>
       </c>
       <c r="BB13">
@@ -3506,7 +3506,7 @@
       <c r="AZ14">
         <v>45</v>
       </c>
-      <c r="BA14">
+      <c r="BA14" s="3">
         <v>40</v>
       </c>
       <c r="BB14">
@@ -3682,7 +3682,7 @@
       <c r="AZ15">
         <v>44</v>
       </c>
-      <c r="BA15">
+      <c r="BA15" s="3">
         <v>39</v>
       </c>
       <c r="BB15">
@@ -3858,7 +3858,7 @@
       <c r="AZ16">
         <v>41</v>
       </c>
-      <c r="BA16">
+      <c r="BA16" s="3">
         <v>40</v>
       </c>
       <c r="BB16">
@@ -4034,7 +4034,7 @@
       <c r="AZ17">
         <v>41</v>
       </c>
-      <c r="BA17">
+      <c r="BA17" s="3">
         <v>40</v>
       </c>
       <c r="BB17">
@@ -4210,7 +4210,7 @@
       <c r="AZ18">
         <v>40</v>
       </c>
-      <c r="BA18">
+      <c r="BA18" s="3">
         <v>39</v>
       </c>
       <c r="BB18">
@@ -4386,7 +4386,7 @@
       <c r="AZ19">
         <v>41</v>
       </c>
-      <c r="BA19">
+      <c r="BA19" s="3">
         <v>38</v>
       </c>
       <c r="BB19">
@@ -4562,7 +4562,7 @@
       <c r="AZ20">
         <v>40</v>
       </c>
-      <c r="BA20">
+      <c r="BA20" s="3">
         <v>42</v>
       </c>
       <c r="BB20">
@@ -4738,7 +4738,7 @@
       <c r="AZ21">
         <v>39</v>
       </c>
-      <c r="BA21">
+      <c r="BA21" s="3">
         <v>43</v>
       </c>
       <c r="BB21">
@@ -4914,7 +4914,7 @@
       <c r="AZ22">
         <v>39</v>
       </c>
-      <c r="BA22">
+      <c r="BA22" s="3">
         <v>43</v>
       </c>
       <c r="BB22">
@@ -5090,7 +5090,7 @@
       <c r="AZ23">
         <v>36</v>
       </c>
-      <c r="BA23">
+      <c r="BA23" s="3">
         <v>42</v>
       </c>
       <c r="BB23">
@@ -5266,7 +5266,7 @@
       <c r="AZ24">
         <v>34</v>
       </c>
-      <c r="BA24">
+      <c r="BA24" s="3">
         <v>42</v>
       </c>
       <c r="BB24">
@@ -5442,7 +5442,7 @@
       <c r="AZ25">
         <v>33</v>
       </c>
-      <c r="BA25">
+      <c r="BA25" s="3">
         <v>54</v>
       </c>
       <c r="BB25">
@@ -5618,7 +5618,7 @@
       <c r="AZ26">
         <v>30</v>
       </c>
-      <c r="BA26">
+      <c r="BA26" s="3">
         <v>58</v>
       </c>
       <c r="BB26">
@@ -5794,7 +5794,7 @@
       <c r="AZ27">
         <v>27</v>
       </c>
-      <c r="BA27">
+      <c r="BA27" s="3">
         <v>53</v>
       </c>
       <c r="BB27">
@@ -5970,7 +5970,7 @@
       <c r="AZ28">
         <v>27</v>
       </c>
-      <c r="BA28">
+      <c r="BA28" s="3">
         <v>53</v>
       </c>
       <c r="BB28">
@@ -6146,7 +6146,7 @@
       <c r="AZ29">
         <v>27</v>
       </c>
-      <c r="BA29">
+      <c r="BA29" s="3">
         <v>52</v>
       </c>
       <c r="BB29">
@@ -6322,7 +6322,7 @@
       <c r="AZ30">
         <v>26</v>
       </c>
-      <c r="BA30">
+      <c r="BA30" s="3">
         <v>52</v>
       </c>
       <c r="BB30">
@@ -6498,7 +6498,7 @@
       <c r="AZ31">
         <v>26</v>
       </c>
-      <c r="BA31">
+      <c r="BA31" s="3">
         <v>52</v>
       </c>
       <c r="BB31">
@@ -6674,7 +6674,7 @@
       <c r="AZ32">
         <v>25</v>
       </c>
-      <c r="BA32">
+      <c r="BA32" s="3">
         <v>52</v>
       </c>
       <c r="BB32">
@@ -6850,7 +6850,7 @@
       <c r="AZ33">
         <v>25</v>
       </c>
-      <c r="BA33">
+      <c r="BA33" s="3">
         <v>52</v>
       </c>
       <c r="BB33">
@@ -7026,7 +7026,7 @@
       <c r="AZ34">
         <v>25</v>
       </c>
-      <c r="BA34">
+      <c r="BA34" s="3">
         <v>53</v>
       </c>
       <c r="BB34">
@@ -7202,7 +7202,7 @@
       <c r="AZ35">
         <v>25</v>
       </c>
-      <c r="BA35">
+      <c r="BA35" s="3">
         <v>53</v>
       </c>
       <c r="BB35">
@@ -7378,7 +7378,7 @@
       <c r="AZ36">
         <v>25</v>
       </c>
-      <c r="BA36">
+      <c r="BA36" s="3">
         <v>49</v>
       </c>
       <c r="BB36">
@@ -7554,7 +7554,7 @@
       <c r="AZ37">
         <v>23</v>
       </c>
-      <c r="BA37">
+      <c r="BA37" s="3">
         <v>48</v>
       </c>
       <c r="BB37">
@@ -7730,7 +7730,7 @@
       <c r="AZ38">
         <v>22</v>
       </c>
-      <c r="BA38">
+      <c r="BA38" s="3">
         <v>47</v>
       </c>
       <c r="BB38">
@@ -7906,7 +7906,7 @@
       <c r="AZ39">
         <v>23</v>
       </c>
-      <c r="BA39">
+      <c r="BA39" s="3">
         <v>47</v>
       </c>
       <c r="BB39">
@@ -8082,7 +8082,7 @@
       <c r="AZ40">
         <v>22</v>
       </c>
-      <c r="BA40">
+      <c r="BA40" s="3">
         <v>47</v>
       </c>
       <c r="BB40">
@@ -8258,7 +8258,7 @@
       <c r="AZ41">
         <v>22</v>
       </c>
-      <c r="BA41">
+      <c r="BA41" s="3">
         <v>71</v>
       </c>
       <c r="BB41">
@@ -8434,7 +8434,7 @@
       <c r="AZ42">
         <v>22</v>
       </c>
-      <c r="BA42">
+      <c r="BA42" s="3">
         <v>65</v>
       </c>
       <c r="BB42">
@@ -8610,7 +8610,7 @@
       <c r="AZ43">
         <v>22</v>
       </c>
-      <c r="BA43">
+      <c r="BA43" s="3">
         <v>65</v>
       </c>
       <c r="BB43">
@@ -8786,7 +8786,7 @@
       <c r="AZ44">
         <v>21</v>
       </c>
-      <c r="BA44">
+      <c r="BA44" s="3">
         <v>65</v>
       </c>
       <c r="BB44">
@@ -8962,7 +8962,7 @@
       <c r="AZ45">
         <v>20</v>
       </c>
-      <c r="BA45">
+      <c r="BA45" s="3">
         <v>69</v>
       </c>
       <c r="BB45">
@@ -9138,7 +9138,7 @@
       <c r="AZ46">
         <v>20</v>
       </c>
-      <c r="BA46">
+      <c r="BA46" s="3">
         <v>69</v>
       </c>
       <c r="BB46">
@@ -9314,7 +9314,7 @@
       <c r="AZ47">
         <v>20</v>
       </c>
-      <c r="BA47">
+      <c r="BA47" s="3">
         <v>84</v>
       </c>
       <c r="BB47">
@@ -9490,7 +9490,7 @@
       <c r="AZ48">
         <v>20</v>
       </c>
-      <c r="BA48">
+      <c r="BA48" s="3">
         <v>89</v>
       </c>
       <c r="BB48">
@@ -9666,7 +9666,7 @@
       <c r="AZ49">
         <v>20</v>
       </c>
-      <c r="BA49">
+      <c r="BA49" s="3">
         <v>86</v>
       </c>
       <c r="BB49">
@@ -9842,7 +9842,7 @@
       <c r="AZ50">
         <v>20</v>
       </c>
-      <c r="BA50">
+      <c r="BA50" s="3">
         <v>61</v>
       </c>
       <c r="BB50">
@@ -10018,7 +10018,7 @@
       <c r="AZ51">
         <v>20</v>
       </c>
-      <c r="BA51">
+      <c r="BA51" s="3">
         <v>62</v>
       </c>
       <c r="BB51">
@@ -10194,7 +10194,7 @@
       <c r="AZ52">
         <v>20</v>
       </c>
-      <c r="BA52">
+      <c r="BA52" s="3">
         <v>62</v>
       </c>
       <c r="BB52">
@@ -10370,7 +10370,7 @@
       <c r="AZ53">
         <v>20</v>
       </c>
-      <c r="BA53">
+      <c r="BA53" s="3">
         <v>62</v>
       </c>
       <c r="BB53">
@@ -10546,7 +10546,7 @@
       <c r="AZ54">
         <v>20</v>
       </c>
-      <c r="BA54">
+      <c r="BA54" s="3">
         <v>62</v>
       </c>
       <c r="BB54">
@@ -10722,7 +10722,7 @@
       <c r="AZ55">
         <v>20</v>
       </c>
-      <c r="BA55">
+      <c r="BA55" s="3">
         <v>62</v>
       </c>
       <c r="BB55">
@@ -10898,7 +10898,7 @@
       <c r="AZ56">
         <v>20</v>
       </c>
-      <c r="BA56">
+      <c r="BA56" s="3">
         <v>60</v>
       </c>
       <c r="BB56">
@@ -11074,7 +11074,7 @@
       <c r="AZ57">
         <v>20</v>
       </c>
-      <c r="BA57">
+      <c r="BA57" s="3">
         <v>59</v>
       </c>
       <c r="BB57">
@@ -11250,7 +11250,7 @@
       <c r="AZ58">
         <v>20</v>
       </c>
-      <c r="BA58">
+      <c r="BA58" s="3">
         <v>65</v>
       </c>
       <c r="BB58">
@@ -11426,7 +11426,7 @@
       <c r="AZ59">
         <v>19</v>
       </c>
-      <c r="BA59">
+      <c r="BA59" s="3">
         <v>65</v>
       </c>
       <c r="BB59">
@@ -11602,7 +11602,7 @@
       <c r="AZ60">
         <v>19</v>
       </c>
-      <c r="BA60">
+      <c r="BA60" s="3">
         <v>91</v>
       </c>
       <c r="BB60">
@@ -11778,7 +11778,7 @@
       <c r="AZ61">
         <v>19</v>
       </c>
-      <c r="BA61">
+      <c r="BA61" s="3">
         <v>65</v>
       </c>
       <c r="BB61">
@@ -11954,7 +11954,7 @@
       <c r="AZ62">
         <v>17</v>
       </c>
-      <c r="BA62">
+      <c r="BA62" s="3">
         <v>65</v>
       </c>
       <c r="BB62">
@@ -12130,7 +12130,7 @@
       <c r="AZ63">
         <v>17</v>
       </c>
-      <c r="BA63">
+      <c r="BA63" s="3">
         <v>65</v>
       </c>
       <c r="BB63">
@@ -12306,7 +12306,7 @@
       <c r="AZ64">
         <v>18</v>
       </c>
-      <c r="BA64">
+      <c r="BA64" s="3">
         <v>63</v>
       </c>
       <c r="BB64">
@@ -12482,7 +12482,7 @@
       <c r="AZ65">
         <v>18</v>
       </c>
-      <c r="BA65">
+      <c r="BA65" s="3">
         <v>63</v>
       </c>
       <c r="BB65">
@@ -12658,7 +12658,7 @@
       <c r="AZ66">
         <v>18</v>
       </c>
-      <c r="BA66">
+      <c r="BA66" s="3">
         <v>63</v>
       </c>
       <c r="BB66">
@@ -12834,7 +12834,7 @@
       <c r="AZ67">
         <v>18</v>
       </c>
-      <c r="BA67">
+      <c r="BA67" s="3">
         <v>62</v>
       </c>
       <c r="BB67">
@@ -13010,7 +13010,7 @@
       <c r="AZ68">
         <v>18</v>
       </c>
-      <c r="BA68">
+      <c r="BA68" s="3">
         <v>62</v>
       </c>
       <c r="BB68">
@@ -13186,7 +13186,7 @@
       <c r="AZ69">
         <v>18</v>
       </c>
-      <c r="BA69">
+      <c r="BA69" s="3">
         <v>62</v>
       </c>
       <c r="BB69">
@@ -13362,7 +13362,7 @@
       <c r="AZ70">
         <v>18</v>
       </c>
-      <c r="BA70">
+      <c r="BA70" s="3">
         <v>60</v>
       </c>
       <c r="BB70">
@@ -13538,7 +13538,7 @@
       <c r="AZ71">
         <v>18</v>
       </c>
-      <c r="BA71">
+      <c r="BA71" s="3">
         <v>58</v>
       </c>
       <c r="BB71">
@@ -13714,7 +13714,7 @@
       <c r="AZ72">
         <v>18</v>
       </c>
-      <c r="BA72">
+      <c r="BA72" s="3">
         <v>55</v>
       </c>
       <c r="BB72">
@@ -13890,7 +13890,7 @@
       <c r="AZ73">
         <v>18</v>
       </c>
-      <c r="BA73">
+      <c r="BA73" s="3">
         <v>55</v>
       </c>
       <c r="BB73">
@@ -14066,7 +14066,7 @@
       <c r="AZ74">
         <v>18</v>
       </c>
-      <c r="BA74">
+      <c r="BA74" s="3">
         <v>55</v>
       </c>
       <c r="BB74">
@@ -14242,7 +14242,7 @@
       <c r="AZ75">
         <v>18</v>
       </c>
-      <c r="BA75">
+      <c r="BA75" s="3">
         <v>54</v>
       </c>
       <c r="BB75">
@@ -14418,7 +14418,7 @@
       <c r="AZ76">
         <v>18</v>
       </c>
-      <c r="BA76">
+      <c r="BA76" s="3">
         <v>54</v>
       </c>
       <c r="BB76">
@@ -14594,7 +14594,7 @@
       <c r="AZ77">
         <v>18</v>
       </c>
-      <c r="BA77">
+      <c r="BA77" s="3">
         <v>57</v>
       </c>
       <c r="BB77">
@@ -14770,7 +14770,7 @@
       <c r="AZ78">
         <v>18</v>
       </c>
-      <c r="BA78">
+      <c r="BA78" s="3">
         <v>57</v>
       </c>
       <c r="BB78">
@@ -14946,7 +14946,7 @@
       <c r="AZ79">
         <v>18</v>
       </c>
-      <c r="BA79">
+      <c r="BA79" s="3">
         <v>56</v>
       </c>
       <c r="BB79">
@@ -15122,7 +15122,7 @@
       <c r="AZ80">
         <v>18</v>
       </c>
-      <c r="BA80">
+      <c r="BA80" s="3">
         <v>58</v>
       </c>
       <c r="BB80">
@@ -15298,7 +15298,7 @@
       <c r="AZ81">
         <v>18</v>
       </c>
-      <c r="BA81">
+      <c r="BA81" s="3">
         <v>58</v>
       </c>
       <c r="BB81">
@@ -15474,7 +15474,7 @@
       <c r="AZ82">
         <v>18</v>
       </c>
-      <c r="BA82">
+      <c r="BA82" s="3">
         <v>55</v>
       </c>
       <c r="BB82">
@@ -15650,7 +15650,7 @@
       <c r="AZ83">
         <v>19</v>
       </c>
-      <c r="BA83">
+      <c r="BA83" s="3">
         <v>62</v>
       </c>
       <c r="BB83">
@@ -15826,7 +15826,7 @@
       <c r="AZ84">
         <v>19</v>
       </c>
-      <c r="BA84">
+      <c r="BA84" s="3">
         <v>62</v>
       </c>
       <c r="BB84">
@@ -16002,7 +16002,7 @@
       <c r="AZ85">
         <v>19</v>
       </c>
-      <c r="BA85">
+      <c r="BA85" s="3">
         <v>90</v>
       </c>
       <c r="BB85">
@@ -16178,7 +16178,7 @@
       <c r="AZ86">
         <v>19</v>
       </c>
-      <c r="BA86">
+      <c r="BA86" s="3">
         <v>88</v>
       </c>
       <c r="BB86">
@@ -16354,7 +16354,7 @@
       <c r="AZ87">
         <v>19</v>
       </c>
-      <c r="BA87">
+      <c r="BA87" s="3">
         <v>88</v>
       </c>
       <c r="BB87">
@@ -16530,7 +16530,7 @@
       <c r="AZ88">
         <v>19</v>
       </c>
-      <c r="BA88">
+      <c r="BA88" s="3">
         <v>82</v>
       </c>
       <c r="BB88">
@@ -16706,7 +16706,7 @@
       <c r="AZ89">
         <v>19</v>
       </c>
-      <c r="BA89">
+      <c r="BA89" s="3">
         <v>83</v>
       </c>
       <c r="BB89">
@@ -16882,7 +16882,7 @@
       <c r="AZ90">
         <v>19</v>
       </c>
-      <c r="BA90">
+      <c r="BA90" s="3">
         <v>83</v>
       </c>
       <c r="BB90">
@@ -17058,7 +17058,7 @@
       <c r="AZ91">
         <v>18</v>
       </c>
-      <c r="BA91">
+      <c r="BA91" s="3">
         <v>83</v>
       </c>
       <c r="BB91">
@@ -17234,7 +17234,7 @@
       <c r="AZ92">
         <v>17</v>
       </c>
-      <c r="BA92">
+      <c r="BA92" s="3">
         <v>82</v>
       </c>
       <c r="BB92">
@@ -17410,7 +17410,7 @@
       <c r="AZ93">
         <v>17</v>
       </c>
-      <c r="BA93">
+      <c r="BA93" s="3">
         <v>66</v>
       </c>
       <c r="BB93">
@@ -17586,7 +17586,7 @@
       <c r="AZ94">
         <v>17</v>
       </c>
-      <c r="BA94">
+      <c r="BA94" s="3">
         <v>66</v>
       </c>
       <c r="BB94">
@@ -17762,7 +17762,7 @@
       <c r="AZ95">
         <v>17</v>
       </c>
-      <c r="BA95">
+      <c r="BA95" s="3">
         <v>66</v>
       </c>
       <c r="BB95">
@@ -17938,7 +17938,7 @@
       <c r="AZ96">
         <v>17</v>
       </c>
-      <c r="BA96">
+      <c r="BA96" s="3">
         <v>50</v>
       </c>
       <c r="BB96">
@@ -18114,7 +18114,7 @@
       <c r="AZ97">
         <v>17</v>
       </c>
-      <c r="BA97">
+      <c r="BA97" s="3">
         <v>50</v>
       </c>
       <c r="BB97">
@@ -18290,7 +18290,7 @@
       <c r="AZ98">
         <v>17</v>
       </c>
-      <c r="BA98">
+      <c r="BA98" s="3">
         <v>50</v>
       </c>
       <c r="BB98">
@@ -18466,7 +18466,7 @@
       <c r="AZ99">
         <v>17</v>
       </c>
-      <c r="BA99">
+      <c r="BA99" s="3">
         <v>50</v>
       </c>
       <c r="BB99">
@@ -18642,7 +18642,7 @@
       <c r="AZ100">
         <v>17</v>
       </c>
-      <c r="BA100">
+      <c r="BA100" s="3">
         <v>49</v>
       </c>
       <c r="BB100">
@@ -18818,7 +18818,7 @@
       <c r="AZ101">
         <v>17</v>
       </c>
-      <c r="BA101">
+      <c r="BA101" s="3">
         <v>49</v>
       </c>
       <c r="BB101">

</xml_diff>